<commit_message>
Reactome network, and pathway lists added
</commit_message>
<xml_diff>
--- a/Cell_Cluster_Annotation_Files/APAP_CTD_Genes.xlsx
+++ b/Cell_Cluster_Annotation_Files/APAP_CTD_Genes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bwanyabrian/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bwanyabrian/Desktop/APAP_scRNA-seq/Cell_Cluster_Annotation_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212D9536-36A6-BD4E-922D-91DDF06C2E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7721C5-526F-6A46-86EF-98C4D20C8323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12580" yWindow="5640" windowWidth="27640" windowHeight="16940" xr2:uid="{1471CD7C-14A7-EB4E-B5DB-FDCF3A7F0F63}"/>
+    <workbookView xWindow="22220" yWindow="6260" windowWidth="27640" windowHeight="16940" xr2:uid="{1471CD7C-14A7-EB4E-B5DB-FDCF3A7F0F63}"/>
   </bookViews>
   <sheets>
     <sheet name="Filtered_APAP_genes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="87">
   <si>
     <t>Chemical Name</t>
   </si>
@@ -194,15 +194,6 @@
     <t>37</t>
   </si>
   <si>
-    <t>ICAM1</t>
-  </si>
-  <si>
-    <t>3383</t>
-  </si>
-  <si>
-    <t>Acetaminophen results in increased expression of ICAM1 mRNA</t>
-  </si>
-  <si>
     <t>IL1B</t>
   </si>
   <si>
@@ -239,15 +230,6 @@
     <t>17</t>
   </si>
   <si>
-    <t>MIR122</t>
-  </si>
-  <si>
-    <t>406906</t>
-  </si>
-  <si>
-    <t>Acetaminophen results in increased expression of MIR122 mRNA</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
@@ -303,6 +285,18 @@
   </si>
   <si>
     <t>36</t>
+  </si>
+  <si>
+    <t>GPT</t>
+  </si>
+  <si>
+    <t>BAX</t>
+  </si>
+  <si>
+    <t>Acetaminophen results in increased expression of BAX mRNA</t>
+  </si>
+  <si>
+    <t>Acetaminophen results in increased expression of GPT mRNA</t>
   </si>
 </sst>
 </file>
@@ -695,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED15414D-E795-AB40-AA75-B07112C2AFA0}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1039,13 +1033,13 @@
         <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>53</v>
+        <v>84</v>
+      </c>
+      <c r="E12" s="2">
+        <v>959</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>15</v>
@@ -1068,19 +1062,19 @@
         <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>22</v>
@@ -1097,19 +1091,19 @@
         <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>17</v>
@@ -1126,19 +1120,19 @@
         <v>11</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>17</v>
@@ -1155,19 +1149,19 @@
         <v>11</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>68</v>
+        <v>83</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4552</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>17</v>
@@ -1184,19 +1178,19 @@
         <v>11</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>17</v>
@@ -1213,13 +1207,13 @@
         <v>11</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>15</v>
@@ -1242,19 +1236,19 @@
         <v>11</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>17</v>
@@ -1271,13 +1265,13 @@
         <v>11</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>15</v>
@@ -1300,19 +1294,19 @@
         <v>11</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>17</v>

</xml_diff>